<commit_message>
gia thue dat nuoc - end
</commit_message>
<xml_diff>
--- a/CSDLGia_ASP/wwwroot/UpLoad/File/DinhGia/Excel/FileExcelGiaThueDN.xlsx
+++ b/CSDLGia_ASP/wwwroot/UpLoad/File/DinhGia/Excel/FileExcelGiaThueDN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CSDLGia_ASP\CSDLGia_ASP\wwwroot\UpLoad\File\DinhGia\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WEB\ASP\CSDLGia_ASP\CSDLGia_ASP\wwwroot\UpLoad\File\DinhGia\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51F3857-6C75-498F-BF9F-4DB6D3AA91BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5EAC77-312E-47EF-AF9C-8F655B344016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6AF4210B-D7D1-451E-A048-5B80F2CEA5CC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6AF4210B-D7D1-451E-A048-5B80F2CEA5CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,46 +25,104 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Vị trí</t>
-  </si>
-  <si>
-    <t>Địa giới từ</t>
-  </si>
-  <si>
-    <t>Địa giới đến</t>
-  </si>
-  <si>
-    <t>Mô tả</t>
-  </si>
-  <si>
-    <t>Diện tích</t>
-  </si>
-  <si>
-    <t>Đơn giá</t>
-  </si>
-  <si>
-    <t>HN</t>
-  </si>
-  <si>
-    <t>HV</t>
-  </si>
-  <si>
-    <t>Đất đồng chũng</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>STT</t>
+  </si>
+  <si>
+    <t>Mã nhóm sản phẩm
+(không có bỏ trống)</t>
+  </si>
+  <si>
+    <t>Vị trí, địa bàn</t>
+  </si>
+  <si>
+    <t>Tỷ lệ %</t>
+  </si>
+  <si>
+    <t>Ngành, nghề đặc biệt ưu đãi đầu tư</t>
+  </si>
+  <si>
+    <t>Ngành, nghề khác</t>
+  </si>
+  <si>
+    <t>Ngành, nghề đặc biệt  đầu tư</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Nhóm đất phi nông nghiệp</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Thành phố Nha Trang</t>
+  </si>
+  <si>
+    <t>Các phường thuộc thành phố Nha Trang</t>
+  </si>
+  <si>
+    <t>Đường loại 1</t>
+  </si>
+  <si>
+    <t>1,1</t>
+  </si>
+  <si>
+    <t>DANH SÁCH GIÁ THUÊ ĐẤT, MẶT NƯỚC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF3F4254"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F4254"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -76,7 +134,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -84,14 +142,68 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -404,63 +516,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD0BC2B6-4560-4170-B0EA-9A729F87B874}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
-    <col min="6" max="6" width="27.140625" customWidth="1"/>
+    <col min="1" max="1" width="19" style="14" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" s="7" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="4" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2">
-        <v>111</v>
-      </c>
-      <c r="F2">
-        <v>5000</v>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="9">
+        <v>1</v>
+      </c>
+      <c r="E7" s="9">
+        <v>1.6</v>
+      </c>
+      <c r="F7" s="9">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:F2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>